<commit_message>
add filter by date
</commit_message>
<xml_diff>
--- a/AlarmReportWeb/dataview/outputs/performance_summary.xlsx
+++ b/AlarmReportWeb/dataview/outputs/performance_summary.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -998,40 +998,40 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
-        <v>44649</v>
+        <v>44647</v>
       </c>
       <c r="B14" t="n">
-        <v>0.15</v>
+        <v>0.119</v>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="D14" t="n">
         <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>0.99</v>
+        <v>0.861</v>
       </c>
       <c r="F14" t="n">
-        <v>0.906</v>
+        <v>0.294</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>0.312</v>
       </c>
       <c r="H14" t="n">
-        <v>0.657</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>0</v>
       </c>
       <c r="J14" t="n">
-        <v>0</v>
+        <v>0.265</v>
       </c>
       <c r="K14" t="n">
-        <v>0.984</v>
+        <v>0.02</v>
       </c>
       <c r="L14" t="n">
-        <v>0.25</v>
+        <v>0.299</v>
       </c>
       <c r="M14" t="n">
         <v>0</v>
@@ -1039,42 +1039,247 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
+        <v>44649</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.906</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>0.657</v>
+      </c>
+      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" t="n">
+        <v>0</v>
+      </c>
+      <c r="K15" t="n">
+        <v>0.984</v>
+      </c>
+      <c r="L15" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="M15" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="n">
         <v>44654</v>
       </c>
-      <c r="B15" t="n">
+      <c r="B16" t="n">
         <v>0.143</v>
       </c>
-      <c r="C15" t="n">
+      <c r="C16" t="n">
         <v>0.001</v>
       </c>
-      <c r="D15" t="n">
-        <v>0</v>
-      </c>
-      <c r="E15" t="n">
+      <c r="D16" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" t="n">
         <v>0.9330000000000001</v>
       </c>
-      <c r="F15" t="n">
+      <c r="F16" t="n">
         <v>0.839</v>
       </c>
-      <c r="G15" t="n">
+      <c r="G16" t="n">
         <v>0.802</v>
       </c>
-      <c r="H15" t="n">
+      <c r="H16" t="n">
         <v>0.833</v>
       </c>
-      <c r="I15" t="n">
+      <c r="I16" t="n">
         <v>0.505</v>
       </c>
-      <c r="J15" t="n">
+      <c r="J16" t="n">
         <v>0.793</v>
       </c>
-      <c r="K15" t="n">
+      <c r="K16" t="n">
         <v>0.985</v>
       </c>
-      <c r="L15" t="n">
+      <c r="L16" t="n">
         <v>0.174</v>
       </c>
-      <c r="M15" t="n">
+      <c r="M16" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="n">
+        <v>44658</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.08599999999999999</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.981</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.518</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.8149999999999999</v>
+      </c>
+      <c r="H17" t="n">
+        <v>0.833</v>
+      </c>
+      <c r="I17" t="n">
+        <v>0.127</v>
+      </c>
+      <c r="J17" t="n">
+        <v>0.728</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.985</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.413</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="n">
+        <v>44659</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.222</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.613</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.711</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0.647</v>
+      </c>
+      <c r="H18" t="n">
+        <v>0.8090000000000001</v>
+      </c>
+      <c r="I18" t="n">
+        <v>0.623</v>
+      </c>
+      <c r="J18" t="n">
+        <v>0.709</v>
+      </c>
+      <c r="K18" t="n">
+        <v>0.979</v>
+      </c>
+      <c r="L18" t="n">
+        <v>0.325</v>
+      </c>
+      <c r="M18" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="n">
+        <v>44660</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.048</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0.044</v>
+      </c>
+      <c r="H19" t="n">
+        <v>0.434</v>
+      </c>
+      <c r="I19" t="n">
+        <v>0</v>
+      </c>
+      <c r="J19" t="n">
+        <v>0</v>
+      </c>
+      <c r="K19" t="n">
+        <v>0.63</v>
+      </c>
+      <c r="L19" t="n">
+        <v>0.333</v>
+      </c>
+      <c r="M19" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="n">
+        <v>44661</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.08799999999999999</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D20" t="n">
+        <v>0</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0.318</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.293</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0.255</v>
+      </c>
+      <c r="H20" t="n">
+        <v>0.226</v>
+      </c>
+      <c r="I20" t="n">
+        <v>0.301</v>
+      </c>
+      <c r="J20" t="n">
+        <v>0.277</v>
+      </c>
+      <c r="K20" t="n">
+        <v>0.308</v>
+      </c>
+      <c r="L20" t="n">
+        <v>0.295</v>
+      </c>
+      <c r="M20" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>